<commit_message>
Updated compounds and scripts, added interpolation details
</commit_message>
<xml_diff>
--- a/Compounds/experiments.xlsx
+++ b/Compounds/experiments.xlsx
@@ -149,7 +149,7 @@
     <t xml:space="preserve">1.45 (I)</t>
   </si>
   <si>
-    <t xml:space="preserve">1.18 (I)</t>
+    <t xml:space="preserve">1.17 (I)</t>
   </si>
   <si>
     <t xml:space="preserve">Table: 2</t>
@@ -511,7 +511,7 @@
     <numFmt numFmtId="167" formatCode="General"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -588,12 +588,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -748,7 +742,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -925,88 +919,72 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1088,11 +1066,11 @@
   </sheetPr>
   <dimension ref="A1:AL1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O61" activeCellId="0" sqref="O61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R105" activeCellId="0" sqref="R105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.28"/>
@@ -1442,10 +1420,10 @@
       </c>
       <c r="N4" s="0" t="n">
         <f aca="false">P4-O4</f>
-        <v>0.443</v>
+        <v>0.433</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="P4" s="24" t="n">
         <v>1.103</v>
@@ -2624,7 +2602,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>-1.57</v>
+        <v>-1.54</v>
       </c>
       <c r="G35" s="41" t="s">
         <v>58</v>
@@ -2745,107 +2723,94 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="37"/>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="45" t="n">
+      <c r="C40" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="D40" s="46" t="n">
-        <v>-1.86</v>
-      </c>
-      <c r="E40" s="46"/>
+      <c r="D40" s="0" t="n">
+        <v>-1.87</v>
+      </c>
       <c r="F40" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G40" s="45" t="s">
+      <c r="G40" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="45" t="s">
+      <c r="H40" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="46" t="s">
+      <c r="K40" s="37"/>
+      <c r="L40" s="0" t="s">
         <v>65</v>
       </c>
       <c r="Z40" s="26"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="37"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="45" t="n">
+      <c r="B41" s="37"/>
+      <c r="C41" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="D41" s="46" t="n">
+      <c r="D41" s="0" t="n">
         <v>-1.53</v>
       </c>
-      <c r="E41" s="46"/>
-      <c r="F41" s="47" t="n">
+      <c r="F41" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="G41" s="45" t="s">
+      <c r="G41" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="48" t="s">
+      <c r="H41" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="49" t="s">
+      <c r="K41" s="37"/>
+      <c r="L41" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="37"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="45" t="n">
+      <c r="B42" s="37"/>
+      <c r="C42" s="38" t="n">
         <v>13</v>
       </c>
-      <c r="D42" s="46" t="n">
+      <c r="D42" s="0" t="n">
         <v>-2.41</v>
       </c>
-      <c r="E42" s="46"/>
-      <c r="F42" s="47" t="n">
+      <c r="F42" s="44" t="n">
         <v>8</v>
       </c>
-      <c r="G42" s="45" t="s">
+      <c r="G42" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="46"/>
+      <c r="K42" s="37"/>
       <c r="Z42" s="26"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="37"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="45" t="n">
+      <c r="B43" s="37"/>
+      <c r="C43" s="38" t="n">
         <v>17.5</v>
       </c>
-      <c r="D43" s="50" t="n">
+      <c r="D43" s="42" t="n">
         <v>-2.9</v>
       </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="47" t="n">
+      <c r="E43" s="42"/>
+      <c r="F43" s="44" t="n">
         <v>9</v>
       </c>
-      <c r="G43" s="45" t="s">
+      <c r="G43" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="46"/>
+      <c r="K43" s="37"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="37" t="s">
@@ -2860,7 +2825,7 @@
       <c r="D45" s="0" t="n">
         <v>-0.26</v>
       </c>
-      <c r="F45" s="51" t="n">
+      <c r="F45" s="46" t="n">
         <v>25</v>
       </c>
       <c r="G45" s="41" t="n">
@@ -2875,7 +2840,7 @@
       </c>
       <c r="J45" s="39" t="n">
         <f aca="false">SQRT(SUMSQ(I45:I48)/COUNTA(I45:I48))</f>
-        <v>0.115542200082913</v>
+        <v>0.120623380818148</v>
       </c>
       <c r="K45" s="37" t="s">
         <v>68</v>
@@ -2890,18 +2855,18 @@
       <c r="D46" s="0" t="n">
         <v>-0.38</v>
       </c>
-      <c r="F46" s="51" t="n">
+      <c r="F46" s="46" t="n">
         <v>25</v>
       </c>
       <c r="G46" s="41" t="n">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="H46" s="41" t="n">
         <v>1.19</v>
       </c>
       <c r="I46" s="0" t="n">
         <f aca="false">H46-G46</f>
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="J46" s="39"/>
       <c r="K46" s="39"/>
@@ -2915,7 +2880,7 @@
       <c r="D47" s="0" t="n">
         <v>-0.55</v>
       </c>
-      <c r="F47" s="51" t="n">
+      <c r="F47" s="46" t="n">
         <v>25</v>
       </c>
       <c r="G47" s="43" t="n">
@@ -2940,18 +2905,18 @@
       <c r="D48" s="0" t="n">
         <v>-0.68</v>
       </c>
-      <c r="F48" s="51" t="n">
+      <c r="F48" s="46" t="n">
         <v>25</v>
       </c>
       <c r="G48" s="43" t="n">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="H48" s="41" t="n">
         <v>1.04</v>
       </c>
       <c r="I48" s="42" t="n">
         <f aca="false">H48-G48</f>
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="J48" s="39"/>
       <c r="K48" s="39"/>
@@ -2963,54 +2928,54 @@
       <c r="B50" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="52" t="n">
+      <c r="C50" s="47" t="n">
         <v>28</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>-2.14</v>
-      </c>
-      <c r="F50" s="53" t="n">
+        <v>-2.15</v>
+      </c>
+      <c r="F50" s="48" t="n">
         <v>4.1</v>
       </c>
-      <c r="G50" s="52" t="n">
+      <c r="G50" s="47" t="n">
         <v>0.66</v>
       </c>
-      <c r="H50" s="52" t="n">
+      <c r="H50" s="47" t="n">
         <v>1.07</v>
       </c>
-      <c r="I50" s="54" t="n">
+      <c r="I50" s="49" t="n">
         <f aca="false">H50-G50</f>
         <v>0.41</v>
       </c>
-      <c r="J50" s="39" t="n">
+      <c r="J50" s="50" t="n">
         <f aca="false">SQRT(SUMSQ(I50:I51)/COUNTA(I50:I51))</f>
-        <v>0.425264623499298</v>
+        <v>0.420119030752</v>
       </c>
       <c r="K50" s="40"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="37"/>
       <c r="B51" s="37"/>
-      <c r="C51" s="52" t="n">
+      <c r="C51" s="47" t="n">
         <v>27.8</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>-2.13</v>
       </c>
-      <c r="F51" s="55" t="n">
+      <c r="F51" s="51" t="n">
         <v>3.7</v>
       </c>
       <c r="G51" s="52" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="H51" s="52" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H51" s="47" t="n">
         <v>1.1</v>
       </c>
-      <c r="I51" s="54" t="n">
+      <c r="I51" s="49" t="n">
         <f aca="false">H51-G51</f>
-        <v>0.44</v>
-      </c>
-      <c r="J51" s="39"/>
+        <v>0.43</v>
+      </c>
+      <c r="J51" s="50"/>
       <c r="K51" s="40"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +2987,7 @@
       <c r="D52" s="0" t="n">
         <v>-0.44</v>
       </c>
-      <c r="F52" s="56" t="n">
+      <c r="F52" s="44" t="n">
         <v>46.3</v>
       </c>
       <c r="G52" s="43" t="n">
@@ -3044,13 +3009,13 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="37"/>
       <c r="B53" s="37"/>
-      <c r="C53" s="57" t="n">
+      <c r="C53" s="53" t="n">
         <v>7</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>-0.56</v>
       </c>
-      <c r="F53" s="56" t="n">
+      <c r="F53" s="44" t="n">
         <v>51.2</v>
       </c>
       <c r="G53" s="41" t="n">
@@ -3078,7 +3043,7 @@
       <c r="D55" s="0" t="n">
         <v>-0.12</v>
       </c>
-      <c r="F55" s="51" t="n">
+      <c r="F55" s="46" t="n">
         <v>75</v>
       </c>
       <c r="G55" s="41" t="n">
@@ -3106,7 +3071,7 @@
       <c r="D56" s="0" t="n">
         <v>-0.23</v>
       </c>
-      <c r="F56" s="51" t="n">
+      <c r="F56" s="46" t="n">
         <v>67</v>
       </c>
       <c r="G56" s="41" t="n">
@@ -3131,7 +3096,7 @@
       <c r="D57" s="0" t="n">
         <v>-0.34</v>
       </c>
-      <c r="F57" s="51" t="n">
+      <c r="F57" s="46" t="n">
         <v>60</v>
       </c>
       <c r="G57" s="43" t="n">
@@ -3156,7 +3121,7 @@
       <c r="D58" s="0" t="n">
         <v>-0.37</v>
       </c>
-      <c r="F58" s="51" t="n">
+      <c r="F58" s="46" t="n">
         <v>59</v>
       </c>
       <c r="G58" s="43" t="n">
@@ -3181,7 +3146,7 @@
       <c r="D59" s="0" t="n">
         <v>-0.44</v>
       </c>
-      <c r="F59" s="51" t="n">
+      <c r="F59" s="46" t="n">
         <v>54</v>
       </c>
       <c r="G59" s="41" t="n">
@@ -3207,7 +3172,7 @@
         <v>-0.5</v>
       </c>
       <c r="E60" s="42"/>
-      <c r="F60" s="51" t="n">
+      <c r="F60" s="46" t="n">
         <v>8</v>
       </c>
       <c r="G60" s="43" t="n">
@@ -3233,7 +3198,7 @@
         <v>-0.6</v>
       </c>
       <c r="E61" s="26"/>
-      <c r="F61" s="51" t="n">
+      <c r="F61" s="46" t="n">
         <v>50</v>
       </c>
       <c r="G61" s="41" t="n">
@@ -3250,10 +3215,10 @@
       <c r="K61" s="39"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="58" t="s">
+      <c r="A63" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="37" t="s">
         <v>22</v>
       </c>
       <c r="C63" s="38" t="n">
@@ -3268,7 +3233,7 @@
       <c r="G63" s="41" t="n">
         <v>2.03</v>
       </c>
-      <c r="H63" s="59" t="s">
+      <c r="H63" s="40" t="s">
         <v>29</v>
       </c>
       <c r="K63" s="0" t="s">
@@ -3276,8 +3241,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="58"/>
-      <c r="B64" s="58"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="38" t="n">
         <v>2.1</v>
       </c>
@@ -3290,11 +3255,11 @@
       <c r="G64" s="41" t="n">
         <v>1.86</v>
       </c>
-      <c r="H64" s="59"/>
+      <c r="H64" s="40"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="58"/>
-      <c r="B65" s="58"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="38" t="n">
         <v>2.4</v>
       </c>
@@ -3307,11 +3272,11 @@
       <c r="G65" s="41" t="n">
         <v>1.81</v>
       </c>
-      <c r="H65" s="59"/>
+      <c r="H65" s="40"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="58"/>
-      <c r="B66" s="58"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
       <c r="C66" s="38" t="n">
         <v>3.7</v>
       </c>
@@ -3324,11 +3289,11 @@
       <c r="G66" s="41" t="n">
         <v>1.69</v>
       </c>
-      <c r="H66" s="59"/>
+      <c r="H66" s="40"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="58"/>
-      <c r="B67" s="58"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="38" t="n">
         <v>4.9</v>
       </c>
@@ -3341,11 +3306,11 @@
       <c r="G67" s="41" t="n">
         <v>1.65</v>
       </c>
-      <c r="H67" s="59"/>
+      <c r="H67" s="40"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="58"/>
-      <c r="B68" s="58"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="38" t="n">
         <v>6.3</v>
       </c>
@@ -3358,11 +3323,11 @@
       <c r="G68" s="41" t="n">
         <v>1.56</v>
       </c>
-      <c r="H68" s="59"/>
+      <c r="H68" s="40"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="58"/>
-      <c r="B69" s="58"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
       <c r="C69" s="38" t="n">
         <v>7.4</v>
       </c>
@@ -3372,14 +3337,14 @@
       <c r="F69" s="38" t="n">
         <v>44</v>
       </c>
-      <c r="G69" s="60" t="n">
+      <c r="G69" s="54" t="n">
         <v>1.5</v>
       </c>
-      <c r="H69" s="59"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="58"/>
-      <c r="B70" s="58"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="38" t="n">
         <v>8.3</v>
       </c>
@@ -3392,12 +3357,12 @@
       <c r="G70" s="41" t="n">
         <v>1.45</v>
       </c>
-      <c r="H70" s="59"/>
+      <c r="H70" s="40"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="58"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="57" t="n">
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="53" t="n">
         <v>12</v>
       </c>
       <c r="D71" s="0" t="n">
@@ -3407,9 +3372,9 @@
         <v>66</v>
       </c>
       <c r="G71" s="41" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="H71" s="59"/>
+        <v>1.17</v>
+      </c>
+      <c r="H71" s="40"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="41"/>
@@ -3481,7 +3446,7 @@
         <v>9.5</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>-2.84</v>
+        <v>-2.85</v>
       </c>
       <c r="F76" s="38" t="n">
         <v>6</v>
@@ -3505,7 +3470,7 @@
         <v>10.9</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>-2.55</v>
+        <v>-2.56</v>
       </c>
       <c r="F77" s="38" t="n">
         <v>5.4</v>
@@ -3536,7 +3501,7 @@
       <c r="F78" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="G78" s="61" t="n">
+      <c r="G78" s="55" t="n">
         <v>0.66</v>
       </c>
       <c r="H78" s="38" t="n">
@@ -3562,7 +3527,7 @@
       <c r="F79" s="38" t="n">
         <v>6.3</v>
       </c>
-      <c r="G79" s="61" t="n">
+      <c r="G79" s="55" t="n">
         <v>1.2</v>
       </c>
       <c r="H79" s="38" t="n">
@@ -3580,11 +3545,11 @@
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="40"/>
       <c r="B80" s="37"/>
-      <c r="C80" s="57" t="n">
+      <c r="C80" s="53" t="n">
         <v>2</v>
       </c>
       <c r="D80" s="26" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="F80" s="38" t="n">
         <v>17</v>
@@ -3632,12 +3597,12 @@
         <v>2.9</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="F82" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G82" s="61" t="n">
+      <c r="G82" s="55" t="n">
         <v>1</v>
       </c>
       <c r="H82" s="38" t="n">
@@ -3652,7 +3617,7 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="40"/>
       <c r="B83" s="37"/>
-      <c r="C83" s="57" t="n">
+      <c r="C83" s="53" t="n">
         <v>5</v>
       </c>
       <c r="D83" s="0" t="n">
@@ -3661,7 +3626,7 @@
       <c r="F83" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G83" s="61" t="n">
+      <c r="G83" s="55" t="n">
         <v>0.82</v>
       </c>
       <c r="H83" s="38" t="n">
@@ -3674,17 +3639,17 @@
       <c r="J83" s="39"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="62" t="s">
+      <c r="C85" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="D85" s="62"/>
-      <c r="E85" s="62"/>
-      <c r="F85" s="62"/>
-      <c r="G85" s="62"/>
-      <c r="H85" s="62"/>
-      <c r="I85" s="62"/>
-      <c r="J85" s="62"/>
-      <c r="K85" s="62"/>
+      <c r="D85" s="56"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="56"/>
+      <c r="H85" s="56"/>
+      <c r="I85" s="56"/>
+      <c r="J85" s="56"/>
+      <c r="K85" s="56"/>
     </row>
     <row r="87" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="29" t="s">
@@ -3849,7 +3814,7 @@
         <v>14</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>-1.57</v>
+        <v>-1.54</v>
       </c>
       <c r="G95" s="41" t="s">
         <v>58</v>
@@ -3969,105 +3934,92 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="37"/>
-      <c r="B100" s="44" t="s">
+      <c r="B100" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C100" s="45" t="n">
+      <c r="C100" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="D100" s="46" t="n">
-        <v>-1.86</v>
-      </c>
-      <c r="E100" s="46"/>
+      <c r="D100" s="0" t="n">
+        <v>-1.87</v>
+      </c>
       <c r="F100" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G100" s="45" t="s">
+      <c r="G100" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H100" s="45" t="s">
+      <c r="H100" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="I100" s="46"/>
-      <c r="J100" s="46"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="46" t="s">
+      <c r="K100" s="37"/>
+      <c r="L100" s="0" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="37"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="45" t="n">
+      <c r="B101" s="37"/>
+      <c r="C101" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="D101" s="46" t="n">
+      <c r="D101" s="0" t="n">
         <v>-1.53</v>
       </c>
-      <c r="E101" s="46"/>
-      <c r="F101" s="47" t="n">
+      <c r="F101" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="G101" s="45" t="s">
+      <c r="G101" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H101" s="48" t="s">
+      <c r="H101" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I101" s="46"/>
-      <c r="J101" s="46"/>
-      <c r="K101" s="44"/>
-      <c r="L101" s="49" t="s">
+      <c r="K101" s="37"/>
+      <c r="L101" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="37"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="45" t="n">
+      <c r="B102" s="37"/>
+      <c r="C102" s="38" t="n">
         <v>13</v>
       </c>
-      <c r="D102" s="46" t="n">
+      <c r="D102" s="0" t="n">
         <v>-2.41</v>
       </c>
-      <c r="E102" s="46"/>
-      <c r="F102" s="47" t="n">
+      <c r="F102" s="44" t="n">
         <v>8</v>
       </c>
-      <c r="G102" s="45" t="s">
+      <c r="G102" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="H102" s="48" t="s">
+      <c r="H102" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I102" s="46"/>
-      <c r="J102" s="46"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="46"/>
+      <c r="K102" s="37"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="37"/>
-      <c r="B103" s="44"/>
-      <c r="C103" s="45" t="n">
+      <c r="B103" s="37"/>
+      <c r="C103" s="38" t="n">
         <v>17.5</v>
       </c>
-      <c r="D103" s="50" t="n">
+      <c r="D103" s="42" t="n">
         <v>-2.9</v>
       </c>
-      <c r="E103" s="50"/>
-      <c r="F103" s="47" t="n">
+      <c r="E103" s="42"/>
+      <c r="F103" s="44" t="n">
         <v>9</v>
       </c>
-      <c r="G103" s="45" t="s">
+      <c r="G103" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="H103" s="48" t="s">
+      <c r="H103" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I103" s="46"/>
-      <c r="J103" s="46"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="46"/>
+      <c r="K103" s="37"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="37" t="s">
@@ -4076,54 +4028,54 @@
       <c r="B105" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="52" t="n">
+      <c r="C105" s="47" t="n">
         <v>28</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>-2.14</v>
-      </c>
-      <c r="F105" s="53" t="n">
+        <v>-2.15</v>
+      </c>
+      <c r="F105" s="48" t="n">
         <v>4.1</v>
       </c>
-      <c r="G105" s="52" t="n">
+      <c r="G105" s="47" t="n">
         <v>0.66</v>
       </c>
-      <c r="H105" s="52" t="n">
+      <c r="H105" s="47" t="n">
         <v>1.07</v>
       </c>
-      <c r="I105" s="54" t="n">
+      <c r="I105" s="49" t="n">
         <f aca="false">H105-G105</f>
         <v>0.41</v>
       </c>
-      <c r="J105" s="39" t="n">
+      <c r="J105" s="50" t="n">
         <f aca="false">SQRT(SUMSQ(I105:I106)/COUNTA(I105:I106))</f>
-        <v>0.425264623499298</v>
+        <v>0.420119030752</v>
       </c>
       <c r="K105" s="40"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="37"/>
       <c r="B106" s="37"/>
-      <c r="C106" s="52" t="n">
+      <c r="C106" s="47" t="n">
         <v>27.8</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>-2.13</v>
       </c>
-      <c r="F106" s="55" t="n">
+      <c r="F106" s="51" t="n">
         <v>3.7</v>
       </c>
       <c r="G106" s="52" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="H106" s="63" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H106" s="57" t="n">
         <v>1.1</v>
       </c>
-      <c r="I106" s="54" t="n">
+      <c r="I106" s="58" t="n">
         <f aca="false">H106-G106</f>
-        <v>0.44</v>
-      </c>
-      <c r="J106" s="39"/>
+        <v>0.43</v>
+      </c>
+      <c r="J106" s="50"/>
       <c r="K106" s="40"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4087,7 @@
       <c r="D107" s="0" t="n">
         <v>-0.44</v>
       </c>
-      <c r="F107" s="56" t="n">
+      <c r="F107" s="44" t="n">
         <v>46.3</v>
       </c>
       <c r="G107" s="43" t="n">
@@ -4163,7 +4115,7 @@
       <c r="D108" s="0" t="n">
         <v>-0.56</v>
       </c>
-      <c r="F108" s="56" t="n">
+      <c r="F108" s="44" t="n">
         <v>51.2</v>
       </c>
       <c r="G108" s="41" t="n">
@@ -4191,7 +4143,7 @@
       <c r="D110" s="0" t="n">
         <v>-0.12</v>
       </c>
-      <c r="F110" s="51" t="n">
+      <c r="F110" s="46" t="n">
         <v>75</v>
       </c>
       <c r="G110" s="41" t="n">
@@ -4204,11 +4156,11 @@
         <f aca="false">H110-G110</f>
         <v>0.05</v>
       </c>
-      <c r="J110" s="39" t="n">
+      <c r="J110" s="50" t="n">
         <f aca="false">SQRT(SUMSQ(I110:I117)/COUNTA(I110:I117))</f>
-        <v>0.101919085553198</v>
-      </c>
-      <c r="K110" s="64" t="s">
+        <v>0.103440804327886</v>
+      </c>
+      <c r="K110" s="37" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4221,7 +4173,7 @@
       <c r="D111" s="0" t="n">
         <v>-0.23</v>
       </c>
-      <c r="F111" s="51" t="n">
+      <c r="F111" s="46" t="n">
         <v>67</v>
       </c>
       <c r="G111" s="41" t="n">
@@ -4234,8 +4186,8 @@
         <f aca="false">H111-G111</f>
         <v>0.0700000000000001</v>
       </c>
-      <c r="J111" s="39"/>
-      <c r="K111" s="39"/>
+      <c r="J111" s="50"/>
+      <c r="K111" s="50"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="37"/>
@@ -4246,7 +4198,7 @@
       <c r="D112" s="0" t="n">
         <v>-0.34</v>
       </c>
-      <c r="F112" s="51" t="n">
+      <c r="F112" s="46" t="n">
         <v>60</v>
       </c>
       <c r="G112" s="43" t="n">
@@ -4259,8 +4211,8 @@
         <f aca="false">H112-G112</f>
         <v>0.0999999999999999</v>
       </c>
-      <c r="J112" s="39"/>
-      <c r="K112" s="39"/>
+      <c r="J112" s="50"/>
+      <c r="K112" s="50"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="37"/>
@@ -4271,7 +4223,7 @@
       <c r="D113" s="0" t="n">
         <v>-0.37</v>
       </c>
-      <c r="F113" s="51" t="n">
+      <c r="F113" s="46" t="n">
         <v>59</v>
       </c>
       <c r="G113" s="43" t="n">
@@ -4284,8 +4236,8 @@
         <f aca="false">H113-G113</f>
         <v>0.0999999999999999</v>
       </c>
-      <c r="J113" s="39"/>
-      <c r="K113" s="39"/>
+      <c r="J113" s="50"/>
+      <c r="K113" s="50"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="37"/>
@@ -4296,7 +4248,7 @@
       <c r="D114" s="0" t="n">
         <v>-0.44</v>
       </c>
-      <c r="F114" s="51" t="n">
+      <c r="F114" s="46" t="n">
         <v>54</v>
       </c>
       <c r="G114" s="41" t="n">
@@ -4309,8 +4261,8 @@
         <f aca="false">H114-G114</f>
         <v>0.1</v>
       </c>
-      <c r="J114" s="39"/>
-      <c r="K114" s="39"/>
+      <c r="J114" s="50"/>
+      <c r="K114" s="50"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="37"/>
@@ -4321,7 +4273,7 @@
       <c r="D115" s="0" t="n">
         <v>-0.55</v>
       </c>
-      <c r="F115" s="51" t="n">
+      <c r="F115" s="46" t="n">
         <v>25</v>
       </c>
       <c r="G115" s="43" t="n">
@@ -4334,8 +4286,8 @@
         <f aca="false">H115-G115</f>
         <v>0.13</v>
       </c>
-      <c r="J115" s="39"/>
-      <c r="K115" s="39"/>
+      <c r="J115" s="50"/>
+      <c r="K115" s="50"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="37"/>
@@ -4347,7 +4299,7 @@
         <v>-0.6</v>
       </c>
       <c r="E116" s="26"/>
-      <c r="F116" s="51" t="n">
+      <c r="F116" s="46" t="n">
         <v>50</v>
       </c>
       <c r="G116" s="41" t="n">
@@ -4360,8 +4312,8 @@
         <f aca="false">H116-G116</f>
         <v>0.12</v>
       </c>
-      <c r="J116" s="39"/>
-      <c r="K116" s="39"/>
+      <c r="J116" s="50"/>
+      <c r="K116" s="50"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="37"/>
@@ -4372,21 +4324,21 @@
       <c r="D117" s="0" t="n">
         <v>-0.68</v>
       </c>
-      <c r="F117" s="51" t="n">
+      <c r="F117" s="46" t="n">
         <v>25</v>
       </c>
-      <c r="G117" s="43" t="n">
-        <v>0.92</v>
+      <c r="G117" s="59" t="n">
+        <v>0.91</v>
       </c>
       <c r="H117" s="41" t="n">
         <v>1.04</v>
       </c>
-      <c r="I117" s="42" t="n">
+      <c r="I117" s="60" t="n">
         <f aca="false">H117-G117</f>
-        <v>0.12</v>
-      </c>
-      <c r="J117" s="39"/>
-      <c r="K117" s="39"/>
+        <v>0.13</v>
+      </c>
+      <c r="J117" s="50"/>
+      <c r="K117" s="50"/>
     </row>
     <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
@@ -4467,7 +4419,7 @@
         <v>9.5</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>-2.84</v>
+        <v>-2.85</v>
       </c>
       <c r="F123" s="38" t="n">
         <v>6</v>
@@ -4491,7 +4443,7 @@
         <v>10.9</v>
       </c>
       <c r="D124" s="0" t="n">
-        <v>-2.55</v>
+        <v>-2.56</v>
       </c>
       <c r="F124" s="38" t="n">
         <v>5.4</v>
@@ -4522,7 +4474,7 @@
       <c r="F125" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="G125" s="61" t="n">
+      <c r="G125" s="55" t="n">
         <v>0.66</v>
       </c>
       <c r="H125" s="38" t="n">
@@ -4548,7 +4500,7 @@
       <c r="F126" s="38" t="n">
         <v>6.3</v>
       </c>
-      <c r="G126" s="61" t="n">
+      <c r="G126" s="55" t="n">
         <v>1.2</v>
       </c>
       <c r="H126" s="38" t="n">
@@ -4566,11 +4518,11 @@
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="40"/>
       <c r="B127" s="37"/>
-      <c r="C127" s="57" t="n">
+      <c r="C127" s="53" t="n">
         <v>2</v>
       </c>
       <c r="D127" s="26" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="F127" s="38" t="n">
         <v>17</v>
@@ -4618,12 +4570,12 @@
         <v>2.9</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="F129" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G129" s="61" t="n">
+      <c r="G129" s="55" t="n">
         <v>1</v>
       </c>
       <c r="H129" s="38" t="n">
@@ -4638,7 +4590,7 @@
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="40"/>
       <c r="B130" s="37"/>
-      <c r="C130" s="57" t="n">
+      <c r="C130" s="53" t="n">
         <v>5</v>
       </c>
       <c r="D130" s="0" t="n">
@@ -4647,7 +4599,7 @@
       <c r="F130" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G130" s="61" t="n">
+      <c r="G130" s="55" t="n">
         <v>0.82</v>
       </c>
       <c r="H130" s="38" t="n">
@@ -4660,17 +4612,17 @@
       <c r="J130" s="39"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="62" t="s">
+      <c r="C132" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="D132" s="62"/>
-      <c r="E132" s="62"/>
-      <c r="F132" s="62"/>
-      <c r="G132" s="62"/>
-      <c r="H132" s="62"/>
-      <c r="I132" s="62"/>
-      <c r="J132" s="62"/>
-      <c r="K132" s="62"/>
+      <c r="D132" s="56"/>
+      <c r="E132" s="56"/>
+      <c r="F132" s="56"/>
+      <c r="G132" s="56"/>
+      <c r="H132" s="56"/>
+      <c r="I132" s="56"/>
+      <c r="J132" s="56"/>
+      <c r="K132" s="56"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4759,8 +4711,8 @@
     <mergeCell ref="C132:K132"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K45" r:id="rId1" display="https://doi.org/10.1063/1.3617461"/>
-    <hyperlink ref="K110" r:id="rId2" display="https://doi.org/10.1063/1.3617461"/>
+    <hyperlink ref="K45" r:id="rId1" display="Appl. Phys. Lett. 99, 042107 (2011); https://doi.org/10.1063/1.3617461"/>
+    <hyperlink ref="K110" r:id="rId2" display="Appl. Phys. Lett. 99, 042107 (2011); https://doi.org/10.1063/1.3617461"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added GaAsPSb bandgap phase diagram
</commit_message>
<xml_diff>
--- a/Compounds/experiments.xlsx
+++ b/Compounds/experiments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="78">
   <si>
     <t xml:space="preserve">Ga(N,As)</t>
   </si>
@@ -497,6 +497,12 @@
     <t xml:space="preserve">Table: 2_new</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage deviation (eV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPD (%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;= 12</t>
   </si>
 </sst>
@@ -504,14 +510,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="General"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -588,6 +595,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -742,7 +755,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -943,18 +956,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -971,20 +976,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1066,11 +1075,11 @@
   </sheetPr>
   <dimension ref="A1:AL1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R105" activeCellId="0" sqref="R105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X119" activeCellId="0" sqref="X119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.28"/>
@@ -1080,7 +1089,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.29"/>
@@ -2947,7 +2956,7 @@
         <f aca="false">H50-G50</f>
         <v>0.41</v>
       </c>
-      <c r="J50" s="50" t="n">
+      <c r="J50" s="39" t="n">
         <f aca="false">SQRT(SUMSQ(I50:I51)/COUNTA(I50:I51))</f>
         <v>0.420119030752</v>
       </c>
@@ -2962,10 +2971,10 @@
       <c r="D51" s="0" t="n">
         <v>-2.13</v>
       </c>
-      <c r="F51" s="51" t="n">
+      <c r="F51" s="50" t="n">
         <v>3.7</v>
       </c>
-      <c r="G51" s="52" t="n">
+      <c r="G51" s="47" t="n">
         <v>0.67</v>
       </c>
       <c r="H51" s="47" t="n">
@@ -2975,7 +2984,7 @@
         <f aca="false">H51-G51</f>
         <v>0.43</v>
       </c>
-      <c r="J51" s="50"/>
+      <c r="J51" s="39"/>
       <c r="K51" s="40"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,7 +3018,7 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="37"/>
       <c r="B53" s="37"/>
-      <c r="C53" s="53" t="n">
+      <c r="C53" s="51" t="n">
         <v>7</v>
       </c>
       <c r="D53" s="0" t="n">
@@ -3337,7 +3346,7 @@
       <c r="F69" s="38" t="n">
         <v>44</v>
       </c>
-      <c r="G69" s="54" t="n">
+      <c r="G69" s="52" t="n">
         <v>1.5</v>
       </c>
       <c r="H69" s="40"/>
@@ -3362,7 +3371,7 @@
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="37"/>
       <c r="B71" s="37"/>
-      <c r="C71" s="53" t="n">
+      <c r="C71" s="51" t="n">
         <v>12</v>
       </c>
       <c r="D71" s="0" t="n">
@@ -3501,7 +3510,7 @@
       <c r="F78" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="G78" s="55" t="n">
+      <c r="G78" s="53" t="n">
         <v>0.66</v>
       </c>
       <c r="H78" s="38" t="n">
@@ -3527,7 +3536,7 @@
       <c r="F79" s="38" t="n">
         <v>6.3</v>
       </c>
-      <c r="G79" s="55" t="n">
+      <c r="G79" s="53" t="n">
         <v>1.2</v>
       </c>
       <c r="H79" s="38" t="n">
@@ -3545,7 +3554,7 @@
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="40"/>
       <c r="B80" s="37"/>
-      <c r="C80" s="53" t="n">
+      <c r="C80" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D80" s="26" t="n">
@@ -3602,7 +3611,7 @@
       <c r="F82" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G82" s="55" t="n">
+      <c r="G82" s="53" t="n">
         <v>1</v>
       </c>
       <c r="H82" s="38" t="n">
@@ -3617,7 +3626,7 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="40"/>
       <c r="B83" s="37"/>
-      <c r="C83" s="53" t="n">
+      <c r="C83" s="51" t="n">
         <v>5</v>
       </c>
       <c r="D83" s="0" t="n">
@@ -3626,7 +3635,7 @@
       <c r="F83" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G83" s="55" t="n">
+      <c r="G83" s="53" t="n">
         <v>0.82</v>
       </c>
       <c r="H83" s="38" t="n">
@@ -3639,17 +3648,17 @@
       <c r="J83" s="39"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="56" t="s">
+      <c r="C85" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="D85" s="56"/>
-      <c r="E85" s="56"/>
-      <c r="F85" s="56"/>
-      <c r="G85" s="56"/>
-      <c r="H85" s="56"/>
-      <c r="I85" s="56"/>
-      <c r="J85" s="56"/>
-      <c r="K85" s="56"/>
+      <c r="D85" s="54"/>
+      <c r="E85" s="54"/>
+      <c r="F85" s="54"/>
+      <c r="G85" s="54"/>
+      <c r="H85" s="54"/>
+      <c r="I85" s="54"/>
+      <c r="J85" s="54"/>
+      <c r="K85" s="54"/>
     </row>
     <row r="87" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="29" t="s">
@@ -3698,6 +3707,12 @@
       </c>
       <c r="L89" s="34" t="s">
         <v>52</v>
+      </c>
+      <c r="M89" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="N89" s="45" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,6 +3732,8 @@
       <c r="J90" s="30"/>
       <c r="K90" s="34"/>
       <c r="L90" s="34"/>
+      <c r="M90" s="30"/>
+      <c r="N90" s="45"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="37" t="s">
@@ -3750,6 +3767,14 @@
       </c>
       <c r="K91" s="40" t="s">
         <v>56</v>
+      </c>
+      <c r="M91" s="55" t="n">
+        <f aca="false">(H91-G91)/H91*100</f>
+        <v>0.602409638554231</v>
+      </c>
+      <c r="N91" s="56" t="n">
+        <f aca="false">SQRT(SUMSQ(M91:M93)/COUNTA(M91:M93))</f>
+        <v>0.478096207589866</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,6 +3801,11 @@
       </c>
       <c r="J92" s="39"/>
       <c r="K92" s="40"/>
+      <c r="M92" s="55" t="n">
+        <f aca="false">(H92-G92)/H92*100</f>
+        <v>0</v>
+      </c>
+      <c r="N92" s="56"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="37"/>
@@ -3802,6 +3832,14 @@
       </c>
       <c r="J93" s="39"/>
       <c r="K93" s="40"/>
+      <c r="M93" s="55" t="n">
+        <f aca="false">(H93-G93)/H93*100</f>
+        <v>0.568181818181819</v>
+      </c>
+      <c r="N93" s="56"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M94" s="55"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="37" t="s">
@@ -3833,6 +3871,14 @@
         <v>60</v>
       </c>
       <c r="L95" s="37"/>
+      <c r="M95" s="55" t="n">
+        <f aca="false">(-0.05)/1.61*100</f>
+        <v>-3.1055900621118</v>
+      </c>
+      <c r="N95" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M95:M99)/COUNTA(M95:M99))</f>
+        <v>11.5440366051117</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="37"/>
@@ -3857,6 +3903,11 @@
       <c r="J96" s="39"/>
       <c r="K96" s="39"/>
       <c r="L96" s="39"/>
+      <c r="M96" s="55" t="n">
+        <f aca="false">(0.06)/1.39*100</f>
+        <v>4.31654676258993</v>
+      </c>
+      <c r="N96" s="57"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="37"/>
@@ -3881,6 +3932,11 @@
       <c r="J97" s="39"/>
       <c r="K97" s="39"/>
       <c r="L97" s="39"/>
+      <c r="M97" s="55" t="n">
+        <f aca="false">(H97-G97)/H97*100</f>
+        <v>0.763358778625955</v>
+      </c>
+      <c r="N97" s="57"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="37"/>
@@ -3905,6 +3961,11 @@
       <c r="J98" s="39"/>
       <c r="K98" s="39"/>
       <c r="L98" s="39"/>
+      <c r="M98" s="55" t="n">
+        <f aca="false">(H98-G98)/H98*100</f>
+        <v>6.76691729323309</v>
+      </c>
+      <c r="N98" s="57"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="37"/>
@@ -3931,6 +3992,11 @@
       <c r="J99" s="39"/>
       <c r="K99" s="39"/>
       <c r="L99" s="39"/>
+      <c r="M99" s="55" t="n">
+        <f aca="false">(H99-G99)/H99*100</f>
+        <v>24.3243243243243</v>
+      </c>
+      <c r="N99" s="57"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="37"/>
@@ -3956,6 +4022,8 @@
       <c r="L100" s="0" t="s">
         <v>65</v>
       </c>
+      <c r="M100" s="55"/>
+      <c r="U100" s="58"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="37"/>
@@ -3979,6 +4047,7 @@
       <c r="L101" s="45" t="s">
         <v>66</v>
       </c>
+      <c r="M101" s="55"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="37"/>
@@ -3999,6 +4068,7 @@
         <v>29</v>
       </c>
       <c r="K102" s="37"/>
+      <c r="M102" s="55"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="37"/>
@@ -4020,6 +4090,10 @@
         <v>29</v>
       </c>
       <c r="K103" s="37"/>
+      <c r="M103" s="55"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M104" s="55"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="37" t="s">
@@ -4047,11 +4121,19 @@
         <f aca="false">H105-G105</f>
         <v>0.41</v>
       </c>
-      <c r="J105" s="50" t="n">
+      <c r="J105" s="39" t="n">
         <f aca="false">SQRT(SUMSQ(I105:I106)/COUNTA(I105:I106))</f>
         <v>0.420119030752</v>
       </c>
       <c r="K105" s="40"/>
+      <c r="M105" s="55" t="n">
+        <f aca="false">(H105-G105)/H105*100</f>
+        <v>38.3177570093458</v>
+      </c>
+      <c r="N105" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M105:M106)/COUNTA(M105:M106))</f>
+        <v>38.7062635485588</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="37"/>
@@ -4062,21 +4144,26 @@
       <c r="D106" s="0" t="n">
         <v>-2.13</v>
       </c>
-      <c r="F106" s="51" t="n">
+      <c r="F106" s="50" t="n">
         <v>3.7</v>
       </c>
-      <c r="G106" s="52" t="n">
+      <c r="G106" s="47" t="n">
         <v>0.67</v>
       </c>
-      <c r="H106" s="57" t="n">
+      <c r="H106" s="59" t="n">
         <v>1.1</v>
       </c>
-      <c r="I106" s="58" t="n">
+      <c r="I106" s="49" t="n">
         <f aca="false">H106-G106</f>
         <v>0.43</v>
       </c>
-      <c r="J106" s="50"/>
+      <c r="J106" s="39"/>
       <c r="K106" s="40"/>
+      <c r="M106" s="55" t="n">
+        <f aca="false">(H106-G106)/H106*100</f>
+        <v>39.0909090909091</v>
+      </c>
+      <c r="N106" s="57"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="37"/>
@@ -4105,6 +4192,14 @@
         <v>0.130384048104053</v>
       </c>
       <c r="K107" s="40"/>
+      <c r="M107" s="55" t="n">
+        <f aca="false">(H107-G107)/H107*100</f>
+        <v>8.95522388059702</v>
+      </c>
+      <c r="N107" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M107:M108)/COUNTA(M107:M108))</f>
+        <v>9.85922140011715</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="37"/>
@@ -4129,6 +4224,16 @@
         <v>0.14</v>
       </c>
       <c r="J108" s="39"/>
+      <c r="M108" s="55" t="n">
+        <f aca="false">(H108-G108)/H108*100</f>
+        <v>10.6870229007634</v>
+      </c>
+      <c r="N108" s="57"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M109" s="55"/>
+      <c r="N109" s="57"/>
+      <c r="U109" s="58"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="37" t="s">
@@ -4156,12 +4261,20 @@
         <f aca="false">H110-G110</f>
         <v>0.05</v>
       </c>
-      <c r="J110" s="50" t="n">
+      <c r="J110" s="39" t="n">
         <f aca="false">SQRT(SUMSQ(I110:I117)/COUNTA(I110:I117))</f>
         <v>0.103440804327886</v>
       </c>
       <c r="K110" s="37" t="s">
         <v>68</v>
+      </c>
+      <c r="M110" s="55" t="n">
+        <f aca="false">(H110-G110)/H110*100</f>
+        <v>3.7593984962406</v>
+      </c>
+      <c r="N110" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M110:M117)/COUNTA(M110:M117))</f>
+        <v>9.23577475730663</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4186,8 +4299,13 @@
         <f aca="false">H111-G111</f>
         <v>0.0700000000000001</v>
       </c>
-      <c r="J111" s="50"/>
-      <c r="K111" s="50"/>
+      <c r="J111" s="39"/>
+      <c r="K111" s="39"/>
+      <c r="M111" s="55" t="n">
+        <f aca="false">(H111-G111)/H111*100</f>
+        <v>5.55555555555556</v>
+      </c>
+      <c r="N111" s="57"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="37"/>
@@ -4211,8 +4329,13 @@
         <f aca="false">H112-G112</f>
         <v>0.0999999999999999</v>
       </c>
-      <c r="J112" s="50"/>
-      <c r="K112" s="50"/>
+      <c r="J112" s="39"/>
+      <c r="K112" s="39"/>
+      <c r="M112" s="55" t="n">
+        <f aca="false">(H112-G112)/H112*100</f>
+        <v>8.33333333333332</v>
+      </c>
+      <c r="N112" s="57"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="37"/>
@@ -4236,8 +4359,13 @@
         <f aca="false">H113-G113</f>
         <v>0.0999999999999999</v>
       </c>
-      <c r="J113" s="50"/>
-      <c r="K113" s="50"/>
+      <c r="J113" s="39"/>
+      <c r="K113" s="39"/>
+      <c r="M113" s="55" t="n">
+        <f aca="false">(H113-G113)/H113*100</f>
+        <v>8.47457627118643</v>
+      </c>
+      <c r="N113" s="57"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="37"/>
@@ -4261,8 +4389,13 @@
         <f aca="false">H114-G114</f>
         <v>0.1</v>
       </c>
-      <c r="J114" s="50"/>
-      <c r="K114" s="50"/>
+      <c r="J114" s="39"/>
+      <c r="K114" s="39"/>
+      <c r="M114" s="55" t="n">
+        <f aca="false">(H114-G114)/H114*100</f>
+        <v>8.77192982456141</v>
+      </c>
+      <c r="N114" s="57"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="37"/>
@@ -4286,8 +4419,13 @@
         <f aca="false">H115-G115</f>
         <v>0.13</v>
       </c>
-      <c r="J115" s="50"/>
-      <c r="K115" s="50"/>
+      <c r="J115" s="39"/>
+      <c r="K115" s="39"/>
+      <c r="M115" s="55" t="n">
+        <f aca="false">(H115-G115)/H115*100</f>
+        <v>11.7117117117117</v>
+      </c>
+      <c r="N115" s="57"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="37"/>
@@ -4312,8 +4450,13 @@
         <f aca="false">H116-G116</f>
         <v>0.12</v>
       </c>
-      <c r="J116" s="50"/>
-      <c r="K116" s="50"/>
+      <c r="J116" s="39"/>
+      <c r="K116" s="39"/>
+      <c r="M116" s="55" t="n">
+        <f aca="false">(H116-G116)/H116*100</f>
+        <v>11.214953271028</v>
+      </c>
+      <c r="N116" s="57"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="37"/>
@@ -4327,18 +4470,27 @@
       <c r="F117" s="46" t="n">
         <v>25</v>
       </c>
-      <c r="G117" s="59" t="n">
+      <c r="G117" s="43" t="n">
         <v>0.91</v>
       </c>
       <c r="H117" s="41" t="n">
         <v>1.04</v>
       </c>
-      <c r="I117" s="60" t="n">
+      <c r="I117" s="42" t="n">
         <f aca="false">H117-G117</f>
         <v>0.13</v>
       </c>
-      <c r="J117" s="50"/>
-      <c r="K117" s="50"/>
+      <c r="J117" s="39"/>
+      <c r="K117" s="39"/>
+      <c r="M117" s="55" t="n">
+        <f aca="false">(H117-G117)/H117*100</f>
+        <v>12.5</v>
+      </c>
+      <c r="N117" s="57"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M118" s="55"/>
+      <c r="N118" s="57"/>
     </row>
     <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
@@ -4348,7 +4500,7 @@
         <v>22</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G119" s="41" t="s">
         <v>29</v>
@@ -4356,6 +4508,12 @@
       <c r="K119" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="M119" s="55"/>
+      <c r="N119" s="57"/>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M120" s="55"/>
+      <c r="N120" s="57"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="40" t="s">
@@ -4387,6 +4545,15 @@
         <f aca="false">SQRT(SUMSQ(I121:I125)/COUNTA(I121:I125))</f>
         <v>0.662314124868253</v>
       </c>
+      <c r="M121" s="55" t="n">
+        <f aca="false">(H121-G121)/H121*100</f>
+        <v>61.1570247933884</v>
+      </c>
+      <c r="N121" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M121:M125)/COUNTA(M121:M125))</f>
+        <v>57.3332814843186</v>
+      </c>
+      <c r="U121" s="58"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="40"/>
@@ -4411,6 +4578,11 @@
         <v>0.71</v>
       </c>
       <c r="J122" s="39"/>
+      <c r="M122" s="55" t="n">
+        <f aca="false">(H122-G122)/H122*100</f>
+        <v>60.6837606837607</v>
+      </c>
+      <c r="N122" s="57"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="40"/>
@@ -4435,6 +4607,11 @@
         <v>0.66</v>
       </c>
       <c r="J123" s="39"/>
+      <c r="M123" s="55" t="n">
+        <f aca="false">(H123-G123)/H123*100</f>
+        <v>59.4594594594595</v>
+      </c>
+      <c r="N123" s="57"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="40"/>
@@ -4459,6 +4636,11 @@
         <v>0.66</v>
       </c>
       <c r="J124" s="39"/>
+      <c r="M124" s="55" t="n">
+        <f aca="false">(H124-G124)/H124*100</f>
+        <v>59.4594594594595</v>
+      </c>
+      <c r="N124" s="57"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="40"/>
@@ -4474,7 +4656,7 @@
       <c r="F125" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="G125" s="55" t="n">
+      <c r="G125" s="53" t="n">
         <v>0.66</v>
       </c>
       <c r="H125" s="38" t="n">
@@ -4485,6 +4667,11 @@
         <v>0.52</v>
       </c>
       <c r="J125" s="39"/>
+      <c r="M125" s="55" t="n">
+        <f aca="false">(H125-G125)/H125*100</f>
+        <v>44.0677966101695</v>
+      </c>
+      <c r="N125" s="57"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="40"/>
@@ -4500,7 +4687,7 @@
       <c r="F126" s="38" t="n">
         <v>6.3</v>
       </c>
-      <c r="G126" s="55" t="n">
+      <c r="G126" s="53" t="n">
         <v>1.2</v>
       </c>
       <c r="H126" s="38" t="n">
@@ -4514,11 +4701,19 @@
         <f aca="false">SQRT(SUMSQ(I126:I130)/COUNTA(I126:I130))</f>
         <v>0.115238882327103</v>
       </c>
+      <c r="M126" s="55" t="n">
+        <f aca="false">(H126-G126)/H126*100</f>
+        <v>4</v>
+      </c>
+      <c r="N126" s="57" t="n">
+        <f aca="false">SQRT(SUMSQ(M126:M130)/COUNTA(M126:M130))</f>
+        <v>10.8003628863081</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="40"/>
       <c r="B127" s="37"/>
-      <c r="C127" s="53" t="n">
+      <c r="C127" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D127" s="26" t="n">
@@ -4538,6 +4733,11 @@
         <v>0.0599999999999998</v>
       </c>
       <c r="J127" s="39"/>
+      <c r="M127" s="55" t="n">
+        <f aca="false">(H127-G127)/H127*100</f>
+        <v>5.17241379310343</v>
+      </c>
+      <c r="N127" s="57"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="40"/>
@@ -4562,6 +4762,11 @@
         <v>0.11</v>
       </c>
       <c r="J128" s="39"/>
+      <c r="M128" s="55" t="n">
+        <f aca="false">(H128-G128)/H128*100</f>
+        <v>9.40170940170939</v>
+      </c>
+      <c r="N128" s="57"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="40"/>
@@ -4575,7 +4780,7 @@
       <c r="F129" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="G129" s="55" t="n">
+      <c r="G129" s="53" t="n">
         <v>1</v>
       </c>
       <c r="H129" s="38" t="n">
@@ -4586,11 +4791,16 @@
         <v>0.11</v>
       </c>
       <c r="J129" s="39"/>
+      <c r="M129" s="55" t="n">
+        <f aca="false">(H129-G129)/H129*100</f>
+        <v>9.90990990990992</v>
+      </c>
+      <c r="N129" s="57"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="40"/>
       <c r="B130" s="37"/>
-      <c r="C130" s="53" t="n">
+      <c r="C130" s="51" t="n">
         <v>5</v>
       </c>
       <c r="D130" s="0" t="n">
@@ -4599,7 +4809,7 @@
       <c r="F130" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G130" s="55" t="n">
+      <c r="G130" s="53" t="n">
         <v>0.82</v>
       </c>
       <c r="H130" s="38" t="n">
@@ -4610,23 +4820,28 @@
         <v>0.19</v>
       </c>
       <c r="J130" s="39"/>
+      <c r="M130" s="55" t="n">
+        <f aca="false">(H130-G130)/H130*100</f>
+        <v>18.8118811881188</v>
+      </c>
+      <c r="N130" s="57"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="56" t="s">
+      <c r="C132" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="D132" s="56"/>
-      <c r="E132" s="56"/>
-      <c r="F132" s="56"/>
-      <c r="G132" s="56"/>
-      <c r="H132" s="56"/>
-      <c r="I132" s="56"/>
-      <c r="J132" s="56"/>
-      <c r="K132" s="56"/>
+      <c r="D132" s="54"/>
+      <c r="E132" s="54"/>
+      <c r="F132" s="54"/>
+      <c r="G132" s="54"/>
+      <c r="H132" s="54"/>
+      <c r="I132" s="54"/>
+      <c r="J132" s="54"/>
+      <c r="K132" s="54"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="91">
     <mergeCell ref="AI3:AI20"/>
     <mergeCell ref="C27:K27"/>
     <mergeCell ref="A29:A30"/>
@@ -4683,14 +4898,18 @@
     <mergeCell ref="J89:J90"/>
     <mergeCell ref="K89:K90"/>
     <mergeCell ref="L89:L90"/>
+    <mergeCell ref="M89:M90"/>
+    <mergeCell ref="N89:N90"/>
     <mergeCell ref="A91:A93"/>
     <mergeCell ref="B91:B93"/>
     <mergeCell ref="J91:J93"/>
     <mergeCell ref="K91:K93"/>
+    <mergeCell ref="N91:N93"/>
     <mergeCell ref="A95:A103"/>
     <mergeCell ref="J95:J99"/>
     <mergeCell ref="K95:K99"/>
     <mergeCell ref="L95:L99"/>
+    <mergeCell ref="N95:N99"/>
     <mergeCell ref="B96:B98"/>
     <mergeCell ref="B100:B103"/>
     <mergeCell ref="K100:K103"/>
@@ -4698,16 +4917,21 @@
     <mergeCell ref="B105:B108"/>
     <mergeCell ref="J105:J106"/>
     <mergeCell ref="K105:K107"/>
+    <mergeCell ref="N105:N106"/>
     <mergeCell ref="J107:J108"/>
+    <mergeCell ref="N107:N108"/>
     <mergeCell ref="A110:A117"/>
     <mergeCell ref="B110:B117"/>
     <mergeCell ref="J110:J117"/>
     <mergeCell ref="K110:K117"/>
+    <mergeCell ref="N110:N117"/>
     <mergeCell ref="A121:A130"/>
     <mergeCell ref="B121:B124"/>
     <mergeCell ref="J121:J125"/>
+    <mergeCell ref="N121:N125"/>
     <mergeCell ref="B126:B130"/>
     <mergeCell ref="J126:J130"/>
+    <mergeCell ref="N126:N130"/>
     <mergeCell ref="C132:K132"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>